<commit_message>
Added the JSON files for data
</commit_message>
<xml_diff>
--- a/Digital-Nurture-4.0-JavaFSE/Java FSE/Deepskilling/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/Digital-Nurture-4.0-JavaFSE/Java FSE/Deepskilling/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/239914_cognizant_com/Documents/2025/Academy work/Digital Nurture/DN 4.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studies\Ragul Files\Deeplearning_upskilling_CTS\Digital-Nurture-4.0-JavaFSE\Java FSE\Deepskilling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{38815D58-CAD9-44C0-B366-FB59C6453CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C9C8729-FA55-40BA-AFF2-34F582845E0A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953218FF-336A-40A5-A265-80CDFB4EA0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
+    <workbookView minimized="1" xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Java FSE" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -829,20 +827,20 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31:F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.08984375" customWidth="1"/>
-    <col min="4" max="4" width="22.6328125" customWidth="1"/>
-    <col min="5" max="5" width="47.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.26953125" customWidth="1"/>
-    <col min="7" max="7" width="30.453125" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="47.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" customWidth="1"/>
+    <col min="7" max="7" width="30.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -861,7 +859,7 @@
       </c>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="18"/>
       <c r="C2" s="16"/>
@@ -878,7 +876,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -897,7 +895,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -916,7 +914,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -935,7 +933,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -954,7 +952,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>2</v>
       </c>
@@ -973,7 +971,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -992,7 +990,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -1011,7 +1009,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>2</v>
       </c>
@@ -1030,7 +1028,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>2</v>
       </c>
@@ -1049,7 +1047,7 @@
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="10"/>
       <c r="C12" s="8"/>
@@ -1060,7 +1058,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>2</v>
       </c>
@@ -1079,7 +1077,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2</v>
       </c>
@@ -1098,7 +1096,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -1117,7 +1115,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>3</v>
       </c>
@@ -1138,7 +1136,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>3</v>
       </c>
@@ -1159,7 +1157,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>3</v>
       </c>
@@ -1180,7 +1178,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>3</v>
       </c>
@@ -1203,7 +1201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>3</v>
       </c>
@@ -1226,7 +1224,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>3</v>
       </c>
@@ -1243,7 +1241,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>3</v>
       </c>
@@ -1260,7 +1258,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>3</v>
       </c>
@@ -1277,7 +1275,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>3</v>
       </c>
@@ -1294,7 +1292,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>4</v>
       </c>
@@ -1317,7 +1315,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>4</v>
       </c>
@@ -1336,7 +1334,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>4</v>
       </c>
@@ -1355,7 +1353,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>4</v>
       </c>
@@ -1374,7 +1372,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>4</v>
       </c>
@@ -1393,7 +1391,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>4</v>
       </c>
@@ -1412,7 +1410,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>5</v>
       </c>
@@ -1435,7 +1433,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="10"/>
       <c r="C32" s="8"/>
@@ -1446,7 +1444,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>6</v>
       </c>
@@ -1469,7 +1467,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>6</v>
       </c>
@@ -1492,7 +1490,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>6</v>
       </c>
@@ -1515,7 +1513,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>6</v>
       </c>
@@ -1534,7 +1532,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>6</v>
       </c>
@@ -1553,7 +1551,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>7</v>
       </c>
@@ -1576,7 +1574,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>7</v>
       </c>
@@ -1599,7 +1597,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>7</v>
       </c>
@@ -1622,7 +1620,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>7</v>
       </c>
@@ -1645,7 +1643,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>7</v>
       </c>
@@ -1668,7 +1666,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>8</v>
       </c>
@@ -1687,7 +1685,7 @@
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>8</v>
       </c>
@@ -1706,7 +1704,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>8</v>
       </c>
@@ -1725,7 +1723,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>8</v>
       </c>
@@ -1744,7 +1742,7 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>8</v>
       </c>
@@ -1765,29 +1763,38 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="C31:C32"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="G11:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2047,15 +2054,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2068,6 +2066,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2083,14 +2089,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>